<commit_message>
sanırım her şey tamam
</commit_message>
<xml_diff>
--- a/MagneticReport.xlsx
+++ b/MagneticReport.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="137" count="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="165" count="666">
   <si>
     <t xml:space="preserve"> GÖZETİM MUAYENE VE EĞİTİM HİZMETLERİ</t>
   </si>
@@ -1522,6 +1522,90 @@
   </si>
   <si>
     <t>32</t>
+  </si>
+  <si>
+    <t>TS EN ISO 17638</t>
+  </si>
+  <si>
+    <t>TS EN ISO 23278 Class B</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>BT-20 LOT:B036P01</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>müş ad</t>
+  </si>
+  <si>
+    <t>Jabbar</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>234</t>
+  </si>
+  <si>
+    <t>sdfs</t>
+  </si>
+  <si>
+    <t>fsfsd</t>
+  </si>
+  <si>
+    <t>fsdfsdfsd</t>
+  </si>
+  <si>
+    <t>İlk deneme</t>
+  </si>
+  <si>
+    <t>gümüşgöze</t>
+  </si>
+  <si>
+    <t>%100</t>
+  </si>
+  <si>
+    <t>son aşama</t>
+  </si>
+  <si>
+    <t>13.06.2020</t>
+  </si>
+  <si>
+    <t>ileri</t>
+  </si>
+  <si>
+    <t>çok</t>
+  </si>
+  <si>
+    <t>e işte</t>
+  </si>
+  <si>
+    <t>yok</t>
+  </si>
+  <si>
+    <t>oki</t>
+  </si>
+  <si>
+    <t>06.2020</t>
+  </si>
+  <si>
+    <t>deneme</t>
+  </si>
+  <si>
+    <t>Hasan</t>
+  </si>
+  <si>
+    <t>biri</t>
+  </si>
+  <si>
+    <t>müdür</t>
+  </si>
+  <si>
+    <t>deniz</t>
   </si>
 </sst>
 </file>
@@ -3945,7 +4029,7 @@
       <c r="B3" s="15"/>
       <c r="C3" s="15"/>
       <c r="D3" t="s" s="16">
-        <v>105</v>
+        <v>142</v>
       </c>
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
@@ -3965,7 +4049,7 @@
       <c r="R3" s="15"/>
       <c r="S3" s="15"/>
       <c r="T3" t="s" s="22">
-        <v>105</v>
+        <v>5</v>
       </c>
       <c r="U3" s="23"/>
       <c r="V3" s="23"/>
@@ -3976,7 +4060,7 @@
       <c r="Y3" s="15"/>
       <c r="Z3" s="15"/>
       <c r="AA3" s="24" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AB3" s="25"/>
     </row>
@@ -3987,7 +4071,7 @@
       <c r="B4" s="27"/>
       <c r="C4" s="28"/>
       <c r="D4" t="s" s="29">
-        <v>105</v>
+        <v>149</v>
       </c>
       <c r="E4" s="30"/>
       <c r="F4" s="30"/>
@@ -4007,7 +4091,7 @@
       <c r="R4" s="27"/>
       <c r="S4" s="27"/>
       <c r="T4" s="32" t="s">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="U4" s="33"/>
       <c r="V4" s="33"/>
@@ -4018,7 +4102,7 @@
       <c r="Y4" s="27"/>
       <c r="Z4" s="27"/>
       <c r="AA4" s="34" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AB4" s="35"/>
     </row>
@@ -4029,7 +4113,7 @@
       <c r="B5" s="27"/>
       <c r="C5" s="27"/>
       <c r="D5" t="s" s="36">
-        <v>105</v>
+        <v>150</v>
       </c>
       <c r="E5" s="37"/>
       <c r="F5" s="38"/>
@@ -4049,7 +4133,7 @@
       <c r="R5" s="27"/>
       <c r="S5" s="27"/>
       <c r="T5" t="s" s="39">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="U5" s="40"/>
       <c r="V5" s="40"/>
@@ -4060,7 +4144,7 @@
       <c r="Y5" s="27"/>
       <c r="Z5" s="27"/>
       <c r="AA5" s="41" t="s">
-        <v>105</v>
+        <v>153</v>
       </c>
       <c r="AB5" s="35"/>
     </row>
@@ -4071,7 +4155,7 @@
       <c r="B6" s="27"/>
       <c r="C6" s="27"/>
       <c r="D6" t="s" s="29">
-        <v>105</v>
+        <v>137</v>
       </c>
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
@@ -4091,7 +4175,7 @@
       <c r="R6" s="27"/>
       <c r="S6" s="27"/>
       <c r="T6" t="s" s="39">
-        <v>105</v>
+        <v>151</v>
       </c>
       <c r="U6" s="40"/>
       <c r="V6" s="40"/>
@@ -4102,7 +4186,7 @@
       <c r="Y6" s="27"/>
       <c r="Z6" s="27"/>
       <c r="AA6" s="34" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AB6" s="35"/>
     </row>
@@ -4113,7 +4197,7 @@
       <c r="B7" s="43"/>
       <c r="C7" s="43"/>
       <c r="D7" t="s" s="44">
-        <v>105</v>
+        <v>138</v>
       </c>
       <c r="E7" s="45"/>
       <c r="F7" s="45"/>
@@ -4133,7 +4217,7 @@
       <c r="R7" s="43"/>
       <c r="S7" s="43"/>
       <c r="T7" t="s" s="47">
-        <v>105</v>
+        <v>152</v>
       </c>
       <c r="U7" s="48"/>
       <c r="V7" s="48"/>
@@ -4144,7 +4228,7 @@
       <c r="Y7" s="43"/>
       <c r="Z7" s="43"/>
       <c r="AA7" t="s" s="44">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AB7" s="49"/>
     </row>
@@ -4188,7 +4272,7 @@
       <c r="C9" s="53"/>
       <c r="D9" s="53"/>
       <c r="E9" t="s" s="54">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="F9" s="55"/>
       <c r="G9" s="55"/>
@@ -4204,7 +4288,7 @@
       <c r="O9" s="53"/>
       <c r="P9" s="53"/>
       <c r="Q9" t="s" s="54">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="R9" s="55"/>
       <c r="S9" s="55"/>
@@ -4217,7 +4301,7 @@
       <c r="X9" s="53"/>
       <c r="Y9" s="53"/>
       <c r="Z9" t="s" s="54">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="AA9" s="55"/>
       <c r="AB9" s="56"/>
@@ -4230,7 +4314,7 @@
       <c r="C10" s="53"/>
       <c r="D10" s="53"/>
       <c r="E10" t="s" s="54">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="F10" s="55"/>
       <c r="G10" s="55"/>
@@ -4246,7 +4330,7 @@
       <c r="O10" s="53"/>
       <c r="P10" s="53"/>
       <c r="Q10" t="s" s="54">
-        <v>105</v>
+        <v>36</v>
       </c>
       <c r="R10" s="55"/>
       <c r="S10" s="55"/>
@@ -4259,7 +4343,7 @@
       <c r="X10" s="58"/>
       <c r="Y10" s="58"/>
       <c r="Z10" t="s" s="54">
-        <v>105</v>
+        <v>38</v>
       </c>
       <c r="AA10" s="55"/>
       <c r="AB10" s="56"/>
@@ -4272,7 +4356,7 @@
       <c r="C11" s="53"/>
       <c r="D11" s="53"/>
       <c r="E11" t="s" s="54">
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="F11" s="55"/>
       <c r="G11" s="55"/>
@@ -4288,7 +4372,7 @@
       <c r="O11" s="53"/>
       <c r="P11" s="53"/>
       <c r="Q11" t="s" s="54">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="R11" s="55"/>
       <c r="S11" s="55"/>
@@ -4299,7 +4383,7 @@
       <c r="X11" s="58"/>
       <c r="Y11" s="58"/>
       <c r="Z11" s="55" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="AA11" s="55"/>
       <c r="AB11" s="56"/>
@@ -4312,7 +4396,7 @@
       <c r="C12" s="53"/>
       <c r="D12" s="53"/>
       <c r="E12" s="55" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="F12" s="59"/>
       <c r="G12" s="59"/>
@@ -4328,7 +4412,7 @@
       <c r="O12" s="53"/>
       <c r="P12" s="53"/>
       <c r="Q12" s="55" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="R12" s="59"/>
       <c r="S12" s="59"/>
@@ -4341,7 +4425,7 @@
       <c r="X12" s="53"/>
       <c r="Y12" s="53"/>
       <c r="Z12" t="s" s="60">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="AA12" s="59"/>
       <c r="AB12" s="61"/>
@@ -4354,7 +4438,7 @@
       <c r="C13" s="53"/>
       <c r="D13" s="53"/>
       <c r="E13" t="s" s="54">
-        <v>105</v>
+        <v>48</v>
       </c>
       <c r="F13" s="55"/>
       <c r="G13" s="55"/>
@@ -4370,7 +4454,7 @@
       <c r="O13" s="53"/>
       <c r="P13" s="53"/>
       <c r="Q13" s="55" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="R13" s="55"/>
       <c r="S13" s="55"/>
@@ -4383,7 +4467,7 @@
       <c r="X13" s="63"/>
       <c r="Y13" s="64"/>
       <c r="Z13" t="s" s="65">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="AA13" s="66"/>
       <c r="AB13" s="67"/>
@@ -4396,7 +4480,7 @@
       <c r="C14" s="68"/>
       <c r="D14" s="68"/>
       <c r="E14" t="s" s="69">
-        <v>105</v>
+        <v>141</v>
       </c>
       <c r="F14" s="70"/>
       <c r="G14" s="70"/>
@@ -4412,7 +4496,7 @@
       <c r="O14" s="68"/>
       <c r="P14" s="68"/>
       <c r="Q14" s="70" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="R14" s="70"/>
       <c r="S14" s="70"/>
@@ -4608,7 +4692,9 @@
       <c r="E20" s="105"/>
       <c r="F20" s="105"/>
       <c r="G20" s="105"/>
-      <c r="H20" s="106"/>
+      <c r="H20" s="106" t="s">
+        <v>157</v>
+      </c>
       <c r="I20" s="107"/>
       <c r="J20" s="107"/>
       <c r="K20" s="107"/>
@@ -4640,7 +4726,9 @@
       <c r="E21" s="110"/>
       <c r="F21" s="110"/>
       <c r="G21" s="110"/>
-      <c r="H21" s="111"/>
+      <c r="H21" s="111" t="s">
+        <v>159</v>
+      </c>
       <c r="I21" s="112"/>
       <c r="J21" s="112"/>
       <c r="K21" s="112"/>
@@ -4672,7 +4760,9 @@
       <c r="E22" s="115"/>
       <c r="F22" s="115"/>
       <c r="G22" s="115"/>
-      <c r="H22" s="96"/>
+      <c r="H22" s="96" t="s">
+        <v>160</v>
+      </c>
       <c r="I22" s="96"/>
       <c r="J22" s="96"/>
       <c r="K22" s="96"/>
@@ -4779,7 +4869,7 @@
         <v>1</v>
       </c>
       <c r="B25" t="s" s="128">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="C25" s="129"/>
       <c r="D25" s="129"/>
@@ -4787,35 +4877,39 @@
       <c r="F25" s="129"/>
       <c r="G25" s="129"/>
       <c r="H25" s="129"/>
-      <c r="I25" s="130">
-        <v>300</v>
+      <c r="I25" s="130" t="s">
+        <v>116</v>
       </c>
       <c r="J25" s="85"/>
       <c r="K25" s="85"/>
       <c r="L25" t="s" s="131">
-        <v>81</v>
+        <v>154</v>
       </c>
       <c r="M25" s="85"/>
       <c r="N25" s="85"/>
       <c r="O25" s="85"/>
       <c r="P25" s="85"/>
       <c r="Q25" s="85"/>
-      <c r="R25" s="130">
-        <v>12</v>
+      <c r="R25" s="130" t="s">
+        <v>155</v>
       </c>
       <c r="S25" t="s" s="131">
-        <v>13</v>
+        <v>156</v>
       </c>
       <c r="T25" s="132"/>
       <c r="U25" s="132"/>
       <c r="V25" s="132"/>
-      <c r="W25" s="133"/>
+      <c r="W25" s="133" t="s">
+        <v>157</v>
+      </c>
       <c r="X25" s="134"/>
-      <c r="Y25" s="85"/>
+      <c r="Y25" s="85" t="s">
+        <v>157</v>
+      </c>
       <c r="Z25" s="85"/>
       <c r="AA25" s="85"/>
       <c r="AB25" t="s" s="135">
-        <v>82</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" ht="21.65" customHeight="1">
@@ -5353,7 +5447,7 @@
       <c r="D40" s="151"/>
       <c r="E40" s="151"/>
       <c r="F40" t="s" s="152">
-        <v>96</v>
+        <v>161</v>
       </c>
       <c r="G40" s="153"/>
       <c r="H40" s="153"/>
@@ -5365,20 +5459,22 @@
       <c r="N40" s="153"/>
       <c r="O40" s="153"/>
       <c r="P40" t="s" s="154">
-        <v>97</v>
+        <v>162</v>
       </c>
       <c r="Q40" s="155"/>
       <c r="R40" s="155"/>
       <c r="S40" s="155"/>
       <c r="T40" s="156"/>
       <c r="U40" t="s" s="154">
-        <v>98</v>
+        <v>163</v>
       </c>
       <c r="V40" s="155"/>
       <c r="W40" s="155"/>
       <c r="X40" s="155"/>
       <c r="Y40" s="156"/>
-      <c r="Z40" s="153"/>
+      <c r="Z40" s="153" t="s">
+        <v>164</v>
+      </c>
       <c r="AA40" s="153"/>
       <c r="AB40" s="157"/>
     </row>
@@ -5391,7 +5487,7 @@
       <c r="D41" s="151"/>
       <c r="E41" s="151"/>
       <c r="F41" t="s" s="158">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="G41" s="30"/>
       <c r="H41" s="30"/>
@@ -5403,20 +5499,22 @@
       <c r="N41" s="30"/>
       <c r="O41" s="30"/>
       <c r="P41" t="s" s="158">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="Q41" s="30"/>
       <c r="R41" s="30"/>
       <c r="S41" s="30"/>
       <c r="T41" s="30"/>
       <c r="U41" t="s" s="152">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="V41" s="153"/>
       <c r="W41" s="153"/>
       <c r="X41" s="153"/>
       <c r="Y41" s="153"/>
-      <c r="Z41" s="153"/>
+      <c r="Z41" s="153" t="s">
+        <v>105</v>
+      </c>
       <c r="AA41" s="153"/>
       <c r="AB41" s="157"/>
     </row>
@@ -5428,8 +5526,8 @@
       <c r="C42" s="151"/>
       <c r="D42" s="151"/>
       <c r="E42" s="151"/>
-      <c r="F42" s="159">
-        <v>43754</v>
+      <c r="F42" s="159" t="s">
+        <v>159</v>
       </c>
       <c r="G42" s="30"/>
       <c r="H42" s="30"/>
@@ -5440,21 +5538,23 @@
       <c r="M42" s="30"/>
       <c r="N42" s="30"/>
       <c r="O42" s="30"/>
-      <c r="P42" s="159">
-        <v>43754</v>
+      <c r="P42" s="159" t="s">
+        <v>159</v>
       </c>
       <c r="Q42" s="30"/>
       <c r="R42" s="30"/>
       <c r="S42" s="30"/>
       <c r="T42" s="30"/>
-      <c r="U42" s="160">
-        <v>43754</v>
+      <c r="U42" s="160" t="s">
+        <v>159</v>
       </c>
       <c r="V42" s="153"/>
       <c r="W42" s="153"/>
       <c r="X42" s="153"/>
       <c r="Y42" s="153"/>
-      <c r="Z42" s="153"/>
+      <c r="Z42" s="153" t="s">
+        <v>159</v>
+      </c>
       <c r="AA42" s="153"/>
       <c r="AB42" s="157"/>
     </row>

</xml_diff>